<commit_message>
fixed issue from feedback
</commit_message>
<xml_diff>
--- a/web/public/data/meta_data.xlsx
+++ b/web/public/data/meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vjz3/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47241D72-DBA0-3A43-8C68-B292099BCB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5D5C3D-BB7E-0645-A927-8D9094BF3EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="30240" windowHeight="19640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="227">
   <si>
     <t>cancer_type</t>
   </si>
@@ -470,9 +470,6 @@
   </si>
   <si>
     <t>pdl1_tissue</t>
-  </si>
-  <si>
-    <t>Keynote246</t>
   </si>
   <si>
     <t>Histology_ClearCell</t>
@@ -1002,7 +999,7 @@
   <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1096,7 +1093,6 @@
       <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
@@ -1501,7 +1497,7 @@
   <dimension ref="A1:Z212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1607,7 +1603,6 @@
       <c r="B12" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1638,7 +1633,6 @@
       <c r="B13" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1669,7 +1663,6 @@
       <c r="B14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1700,7 +1693,6 @@
       <c r="B15" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1731,7 +1723,6 @@
       <c r="B16" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1765,7 +1756,6 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1796,7 +1786,6 @@
       <c r="B18" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1827,7 +1816,6 @@
       <c r="B19" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1858,7 +1846,6 @@
       <c r="B20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1889,7 +1876,6 @@
       <c r="B21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1920,7 +1906,6 @@
       <c r="B22" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -3077,15 +3062,15 @@
     </row>
     <row r="158" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A158" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B158" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B159" s="4" t="s">
         <v>107</v>
@@ -3096,7 +3081,7 @@
     </row>
     <row r="160" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A160" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B160" s="4" t="s">
         <v>106</v>
@@ -3104,7 +3089,7 @@
     </row>
     <row r="161" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A161" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B161" s="4" t="s">
         <v>104</v>
@@ -3112,7 +3097,7 @@
     </row>
     <row r="162" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B162" s="4" t="s">
         <v>108</v>
@@ -3120,7 +3105,7 @@
     </row>
     <row r="163" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B163" s="4" t="s">
         <v>109</v>
@@ -3128,7 +3113,7 @@
     </row>
     <row r="164" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A164" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B164" s="4" t="s">
         <v>110</v>
@@ -3136,7 +3121,7 @@
     </row>
     <row r="165" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B165" s="4" t="s">
         <v>112</v>
@@ -3144,7 +3129,7 @@
     </row>
     <row r="166" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A166" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B166" s="4" t="s">
         <v>111</v>
@@ -3152,7 +3137,7 @@
     </row>
     <row r="167" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A167" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B167" s="4" t="s">
         <v>113</v>
@@ -3160,7 +3145,7 @@
     </row>
     <row r="168" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B168" s="4" t="s">
         <v>119</v>
@@ -3168,15 +3153,15 @@
     </row>
     <row r="169" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A170" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B170" s="4" t="s">
         <v>140</v>
@@ -3184,7 +3169,7 @@
     </row>
     <row r="171" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="4" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B171" s="4" t="s">
         <v>128</v>
@@ -3286,7 +3271,7 @@
         <v>89</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -3462,9 +3447,7 @@
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3476,10 +3459,10 @@
         <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3487,10 +3470,10 @@
         <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3498,10 +3481,10 @@
         <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3509,10 +3492,10 @@
         <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3520,10 +3503,10 @@
         <v>107</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3531,10 +3514,10 @@
         <v>108</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3542,10 +3525,10 @@
         <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3553,10 +3536,10 @@
         <v>110</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3564,10 +3547,10 @@
         <v>111</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3575,10 +3558,10 @@
         <v>112</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3586,10 +3569,10 @@
         <v>113</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3597,10 +3580,10 @@
         <v>114</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3608,10 +3591,10 @@
         <v>115</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3619,10 +3602,10 @@
         <v>116</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3630,10 +3613,10 @@
         <v>117</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3641,10 +3624,10 @@
         <v>118</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3652,10 +3635,10 @@
         <v>119</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3663,10 +3646,10 @@
         <v>120</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3674,10 +3657,10 @@
         <v>121</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3685,10 +3668,10 @@
         <v>122</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3696,10 +3679,10 @@
         <v>123</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3707,10 +3690,10 @@
         <v>124</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3718,10 +3701,10 @@
         <v>125</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3729,10 +3712,10 @@
         <v>126</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3740,10 +3723,10 @@
         <v>127</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3751,10 +3734,10 @@
         <v>128</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3762,10 +3745,10 @@
         <v>129</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3773,10 +3756,10 @@
         <v>130</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3784,10 +3767,10 @@
         <v>131</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3795,10 +3778,10 @@
         <v>132</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3806,10 +3789,10 @@
         <v>133</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3817,10 +3800,10 @@
         <v>134</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3828,10 +3811,10 @@
         <v>135</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3839,10 +3822,10 @@
         <v>136</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3850,10 +3833,10 @@
         <v>137</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3861,10 +3844,10 @@
         <v>138</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3872,10 +3855,10 @@
         <v>139</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3883,10 +3866,10 @@
         <v>140</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3894,10 +3877,10 @@
         <v>141</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3905,10 +3888,10 @@
         <v>142</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3916,10 +3899,10 @@
         <v>143</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3927,10 +3910,10 @@
         <v>145</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3938,10 +3921,10 @@
         <v>146</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3949,10 +3932,10 @@
         <v>147</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3960,32 +3943,32 @@
         <v>148</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -4001,7 +3984,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" activeCellId="1" sqref="H27 C36"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4018,42 +4001,42 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" s="1">
         <v>0.77</v>
@@ -4085,10 +4068,10 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="C3" s="1">
         <v>0.75</v>
@@ -4120,10 +4103,10 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C4" s="1">
         <v>0.73</v>
@@ -4155,10 +4138,10 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C5" s="1">
         <v>0.71</v>
@@ -4190,10 +4173,10 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" s="1">
         <v>0.69</v>
@@ -4225,10 +4208,10 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C7" s="1">
         <v>0.67</v>
@@ -4260,10 +4243,10 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8" s="1">
         <v>0.65</v>
@@ -4295,10 +4278,10 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C9" s="1">
         <v>0.63</v>
@@ -4330,10 +4313,10 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C10" s="1">
         <v>0.61</v>
@@ -4365,10 +4348,10 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C11" s="1">
         <v>0.59</v>
@@ -4400,10 +4383,10 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C12" s="1">
         <v>0.56999999999999995</v>
@@ -4435,10 +4418,10 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C13" s="1">
         <v>0.55000000000000004</v>
@@ -4470,10 +4453,10 @@
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C14" s="1">
         <v>0.53</v>
@@ -4505,10 +4488,10 @@
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C15" s="1">
         <v>0.51</v>
@@ -4540,10 +4523,10 @@
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C16" s="1">
         <v>0.49</v>

</xml_diff>